<commit_message>
firstDraft and updated results and research
adding Kevin research and updating marlene results
Also added complete rough/first draft
</commit_message>
<xml_diff>
--- a/FinalExcelwithCharts/Result.xlsx
+++ b/FinalExcelwithCharts/Result.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="195" windowWidth="21075" windowHeight="8775"/>
+    <workbookView xWindow="210" yWindow="195" windowWidth="21075" windowHeight="8775" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Result2" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Charts" sheetId="2" r:id="rId3"/>
     <sheet name="Distance Prediction" sheetId="4" r:id="rId4"/>
     <sheet name="Kevin's Tests" sheetId="5" r:id="rId5"/>
+    <sheet name="Marlene's Tests" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="29">
   <si>
     <t>Method</t>
   </si>
@@ -2463,11 +2464,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="122739200"/>
-        <c:axId val="122637120"/>
+        <c:axId val="132253184"/>
+        <c:axId val="132403136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="122739200"/>
+        <c:axId val="132253184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2509,7 +2510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122637120"/>
+        <c:crossAx val="132403136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2517,7 +2518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122637120"/>
+        <c:axId val="132403136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,7 +2568,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122739200"/>
+        <c:crossAx val="132253184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5907,7 +5908,7 @@
   </sheetPr>
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -6604,4 +6605,152 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>19</v>
+      </c>
+      <c r="D2">
+        <v>32</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>28</v>
+      </c>
+      <c r="H2">
+        <v>3.1157399999999998E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>0.64671900000000004</v>
+      </c>
+      <c r="C3">
+        <v>0.70674199999999998</v>
+      </c>
+      <c r="D3">
+        <v>0.47647499999999998</v>
+      </c>
+      <c r="E3">
+        <v>0.85464099999999998</v>
+      </c>
+      <c r="F3">
+        <v>0.84947399999999995</v>
+      </c>
+      <c r="G3">
+        <v>0.60762000000000005</v>
+      </c>
+      <c r="H3">
+        <v>1.5578699999999999E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>44</v>
+      </c>
+      <c r="F4">
+        <v>33</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>3.1157399999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>-21</v>
+      </c>
+      <c r="C5">
+        <v>-6</v>
+      </c>
+      <c r="D5">
+        <v>-47</v>
+      </c>
+      <c r="E5">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>-9</v>
+      </c>
+      <c r="G5">
+        <v>-12</v>
+      </c>
+      <c r="H5">
+        <v>4.6736100000000003E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Excel with Charts
I ran both data files, two more times in order to average my runs.
</commit_message>
<xml_diff>
--- a/FinalExcelwithCharts/Result.xlsx
+++ b/FinalExcelwithCharts/Result.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="34">
   <si>
     <t>Method</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>Emily Dickenson's poem</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average </t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -695,7 +704,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -959,7 +967,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1051,7 +1058,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1314,7 +1320,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1406,7 +1411,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1669,7 +1673,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1761,7 +1764,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2025,7 +2027,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2148,7 +2149,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2509,11 +2509,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="317161328"/>
-        <c:axId val="317161720"/>
+        <c:axId val="246522264"/>
+        <c:axId val="246522656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="317161328"/>
+        <c:axId val="246522264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2544,7 +2544,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2609,7 +2608,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317161720"/>
+        <c:crossAx val="246522656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2617,7 +2616,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="317161720"/>
+        <c:axId val="246522656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2663,7 +2662,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2722,7 +2720,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="317161328"/>
+        <c:crossAx val="246522264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2737,7 +2735,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6765,10 +6762,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6776,12 +6773,12 @@
     <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -6816,10 +6813,19 @@
         <v>27</v>
       </c>
       <c r="L2" t="s">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -6856,8 +6862,18 @@
       <c r="L3">
         <v>4.6423199999999998E-2</v>
       </c>
+      <c r="M3">
+        <v>5.46875E-2</v>
+      </c>
+      <c r="N3">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="O3">
+        <f>AVERAGE(L3:N3)</f>
+        <v>4.6724399999999999E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -6894,8 +6910,18 @@
       <c r="L4">
         <v>1.5474399999999999E-2</v>
       </c>
+      <c r="M4">
+        <v>2.34375E-2</v>
+      </c>
+      <c r="N4">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O6" si="0">AVERAGE(L4:N4)</f>
+        <v>1.8178966666666668E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -6932,8 +6958,18 @@
       <c r="L5">
         <v>7.7371999999999996E-3</v>
       </c>
+      <c r="M5">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="N5">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>1.0391566666666666E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -6970,13 +7006,23 @@
       <c r="L6">
         <v>3.8685999999999998E-2</v>
       </c>
+      <c r="M6">
+        <v>3.125E-2</v>
+      </c>
+      <c r="N6">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>3.6332833333333335E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -6990,10 +7036,19 @@
         <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -7009,8 +7064,18 @@
       <c r="E10">
         <v>3.8928999999999998E-2</v>
       </c>
+      <c r="F10">
+        <v>3.90625E-2</v>
+      </c>
+      <c r="G10">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H10">
+        <f>AVERAGE(E10:G10)</f>
+        <v>3.6413833333333333E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -7026,8 +7091,18 @@
       <c r="E11">
         <v>7.7857999999999998E-3</v>
       </c>
+      <c r="F11">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G11">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H13" si="1">AVERAGE(E11:G11)</f>
+        <v>7.8035999999999999E-3</v>
+      </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -7043,8 +7118,18 @@
       <c r="E12">
         <v>7.7857999999999998E-3</v>
       </c>
+      <c r="F12">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="G12">
+        <v>7.8125E-3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>7.8035999999999999E-3</v>
+      </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -7059,6 +7144,16 @@
       </c>
       <c r="E13">
         <v>2.33574E-2</v>
+      </c>
+      <c r="F13">
+        <v>2.34375E-2</v>
+      </c>
+      <c r="G13">
+        <v>2.34375E-2</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>2.3410799999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated Kevin results tab
updated Kevin results tab
</commit_message>
<xml_diff>
--- a/FinalExcelwithCharts/Result.xlsx
+++ b/FinalExcelwithCharts/Result.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlclab\Documents\GitHub\DigitalHumanities\FinalExcelwithCharts\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="210" yWindow="195" windowWidth="21075" windowHeight="8775" activeTab="1"/>
+    <workbookView xWindow="210" yWindow="195" windowWidth="21075" windowHeight="8775" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Result2" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
     <sheet name="Kevin's Tests" sheetId="5" r:id="rId5"/>
     <sheet name="Marlene's Tests" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -2157,32 +2152,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:effectLst>
-                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                  <a:prstClr val="black">
-                    <a:alpha val="40000"/>
-                  </a:prstClr>
-                </a:outerShdw>
-              </a:effectLst>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2509,11 +2478,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="246522264"/>
-        <c:axId val="246522656"/>
+        <c:axId val="137968128"/>
+        <c:axId val="138105344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246522264"/>
+        <c:axId val="137968128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2552,25 +2521,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -2608,7 +2558,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246522656"/>
+        <c:crossAx val="138105344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2616,7 +2566,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246522656"/>
+        <c:axId val="138105344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -2670,25 +2620,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="85000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -2720,7 +2651,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="246522264"/>
+        <c:crossAx val="137968128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -5812,7 +5743,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5847,7 +5778,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6308,7 +6239,7 @@
   </sheetPr>
   <dimension ref="A2:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="E3:H3"/>
     </sheetView>
   </sheetViews>
@@ -6510,8 +6441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="A1:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6598,17 +6529,17 @@
         <v>10</v>
       </c>
       <c r="L2">
-        <v>0.15626300000000001</v>
+        <v>0.154304</v>
       </c>
       <c r="M2">
-        <v>0.15626799999999999</v>
+        <v>0.164076</v>
       </c>
       <c r="N2">
-        <v>0.15656900000000001</v>
+        <v>0.165051</v>
       </c>
       <c r="O2">
         <f>AVERAGE(L2:N2)</f>
-        <v>0.15636666666666668</v>
+        <v>0.16114366666666666</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -6646,17 +6577,17 @@
         <v>0.89908699999999997</v>
       </c>
       <c r="L3">
-        <v>6.2498100000000001E-2</v>
+        <v>2.2464000000000001E-2</v>
       </c>
       <c r="M3">
-        <v>1.5626600000000001E-2</v>
+        <v>6.3476199999999997E-2</v>
       </c>
       <c r="N3">
-        <v>1.53198E-2</v>
+        <v>6.2502299999999997E-2</v>
       </c>
       <c r="O3">
         <f t="shared" ref="O3:O5" si="0">AVERAGE(L3:N3)</f>
-        <v>3.1148166666666668E-2</v>
+        <v>4.9480833333333328E-2</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -6664,47 +6595,47 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="C4">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="E4">
         <v>109</v>
       </c>
       <c r="F4">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="G4">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="H4">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="I4">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="J4">
-        <v>112</v>
+        <v>52</v>
       </c>
       <c r="K4">
-        <v>113</v>
+        <v>52</v>
       </c>
       <c r="L4">
-        <v>4.6872999999999998E-2</v>
+        <v>2.44218E-2</v>
       </c>
       <c r="M4">
-        <v>3.1246699999999999E-2</v>
+        <v>6.1529300000000002E-2</v>
       </c>
       <c r="N4">
-        <v>3.1252599999999998E-2</v>
+        <v>3.6135E-2</v>
       </c>
       <c r="O4">
         <f t="shared" si="0"/>
-        <v>3.6457433333333338E-2</v>
+        <v>4.069536666666667E-2</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -6742,17 +6673,17 @@
         <v>84</v>
       </c>
       <c r="L5">
-        <v>0.109378</v>
+        <v>0.112313</v>
       </c>
       <c r="M5">
-        <v>9.3757099999999996E-2</v>
+        <v>0.11622</v>
       </c>
       <c r="N5">
-        <v>0.109384</v>
+        <v>0.108406</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>0.10417303333333333</v>
+        <v>0.112313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>